<commit_message>
import excel màn học viên
</commit_message>
<xml_diff>
--- a/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
+++ b/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE8388F-9F34-49A1-BD9E-6F2478BB82D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC9382D-9A41-491C-A594-80254A574D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fixbug: import học viên
</commit_message>
<xml_diff>
--- a/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
+++ b/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC9382D-9A41-491C-A594-80254A574D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD0837D-CBE3-431F-97B3-7AED7D01CA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1380" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HocVien" sheetId="1" r:id="rId1"/>
+    <sheet name="ChuyenNghanh" sheetId="2" r:id="rId2"/>
+    <sheet name="NhaKhoaHoc" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
-  <si>
-    <t>Các cột màu cam là thông tin bắt buộc nhập</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -55,58 +54,55 @@
     <t>Ngày sinh</t>
   </si>
   <si>
+    <t>Hướng dẫn một</t>
+  </si>
+  <si>
+    <t>Hướng dẫn hai</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>HV001</t>
+  </si>
+  <si>
+    <t>Tên học viên</t>
+  </si>
+  <si>
+    <t>Trần Quốc Bình</t>
+  </si>
+  <si>
+    <t>binhtq@gmail.com</t>
+  </si>
+  <si>
+    <t>0919083644</t>
+  </si>
+  <si>
+    <t>20/10/2002</t>
+  </si>
+  <si>
+    <t>Chuyên nghành</t>
+  </si>
+  <si>
+    <t>InstructorIdOne</t>
+  </si>
+  <si>
+    <t>InstructorIdTwo</t>
+  </si>
+  <si>
+    <t>SpecializedId</t>
+  </si>
+  <si>
+    <t>TopicName</t>
+  </si>
+  <si>
     <t>Tên đề tài</t>
-  </si>
-  <si>
-    <t>Hướng dẫn một</t>
-  </si>
-  <si>
-    <t>Hướng dẫn hai</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>TopicName</t>
-  </si>
-  <si>
-    <t>InstructorOne</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>HV001</t>
-  </si>
-  <si>
-    <t>Tên học viên</t>
-  </si>
-  <si>
-    <t>Trần Quốc Bình</t>
-  </si>
-  <si>
-    <t>binhtq@gmail.com</t>
-  </si>
-  <si>
-    <t>0919083644</t>
-  </si>
-  <si>
-    <t>20/10/2002</t>
-  </si>
-  <si>
-    <t>Bảo vệ môi trường</t>
-  </si>
-  <si>
-    <t>Đinh Thanh Trung</t>
-  </si>
-  <si>
-    <t>Hoàng Thanh Tùng</t>
-  </si>
-  <si>
-    <t>OnstructorTwo</t>
   </si>
 </sst>
 </file>
@@ -160,24 +156,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -191,8 +175,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -225,19 +215,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -260,19 +237,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -308,48 +272,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -658,164 +620,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="3" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="23" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="24.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="23" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="12"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6 F6">
+  <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>#REF!="Thử việc"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6 F6">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF!="nghỉ việc"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6 F6">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>#REF!="thai sản"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{BD313D4A-5793-4918-ABF3-E5E099E009F1}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{6801BDB6-C5A3-4F7E-97B8-1CC42AEA7525}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{462E3BC5-EF01-43BD-BEA9-EEB43D96B046}">
+          <x14:formula1>
+            <xm:f>NhaKhoaHoc!$A$4:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>I6:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF448049-A736-4BB2-8107-28BE25E0A91C}">
+          <x14:formula1>
+            <xm:f>ChuyenNghanh!$B$4:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>G6:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB2454B-335C-424A-BC73-23D3115D1C15}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F94C13A-83D2-4941-AEB3-734DDB965E02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fxibug: sai tên sheet
</commit_message>
<xml_diff>
--- a/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
+++ b/luanvanthacsi/Excel/Template/DanhSachHocVien.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="HocVien" sheetId="1" r:id="rId1"/>
-    <sheet name="ChuyenNghanh" sheetId="2" r:id="rId2"/>
+    <sheet name="ChuyenNganh" sheetId="2" r:id="rId2"/>
     <sheet name="NhaKhoaHoc" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -784,7 +784,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ChuyenNghanh!$B$4:$B$1048576</xm:f>
+            <xm:f>ChuyenNganh!$B$4:$B$1048576</xm:f>
           </x14:formula1>
           <xm:sqref>G6:G1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>